<commit_message>
update daily doodth file nov 25, 2021
</commit_message>
<xml_diff>
--- a/2021/november,  2021.xlsx
+++ b/2021/november,  2021.xlsx
@@ -669,8 +669,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:BD39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="Z1" workbookViewId="0">
-      <selection activeCell="AK25" sqref="AK25"/>
+    <sheetView tabSelected="1" topLeftCell="AR1" workbookViewId="0">
+      <selection activeCell="BB26" sqref="BB26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -4769,66 +4769,154 @@
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="H26" s="7"/>
-      <c r="I26" s="7"/>
-      <c r="J26" s="7"/>
-      <c r="K26" s="7"/>
-      <c r="L26" s="7"/>
-      <c r="M26" s="7"/>
-      <c r="N26" s="7"/>
-      <c r="O26" s="7"/>
-      <c r="P26" s="7"/>
-      <c r="Q26" s="7"/>
-      <c r="R26" s="7"/>
-      <c r="S26" s="7"/>
-      <c r="T26" s="7"/>
-      <c r="U26" s="7"/>
-      <c r="V26" s="7"/>
-      <c r="W26" s="7"/>
-      <c r="X26" s="7"/>
-      <c r="Y26" s="7"/>
-      <c r="Z26" s="7"/>
-      <c r="AA26" s="7"/>
-      <c r="AB26" s="7"/>
-      <c r="AC26" s="7"/>
-      <c r="AD26" s="7"/>
-      <c r="AE26" s="7"/>
-      <c r="AF26" s="7"/>
-      <c r="AG26" s="7"/>
-      <c r="AH26" s="7"/>
-      <c r="AI26" s="7"/>
-      <c r="AJ26" s="7"/>
-      <c r="AK26" s="7"/>
-      <c r="AL26" s="7"/>
-      <c r="AM26" s="7"/>
-      <c r="AN26" s="7"/>
-      <c r="AO26" s="7"/>
-      <c r="AP26" s="7"/>
-      <c r="AQ26" s="7"/>
-      <c r="AR26" s="7"/>
-      <c r="AS26" s="7"/>
-      <c r="AT26" s="7"/>
-      <c r="AU26" s="7"/>
-      <c r="AV26" s="7"/>
-      <c r="AW26" s="7"/>
-      <c r="AX26" s="7"/>
-      <c r="AY26" s="28"/>
+      <c r="H26" s="7">
+        <v>0.5</v>
+      </c>
+      <c r="I26" s="7">
+        <v>3</v>
+      </c>
+      <c r="J26" s="7">
+        <v>1.5</v>
+      </c>
+      <c r="K26" s="7">
+        <v>2</v>
+      </c>
+      <c r="L26" s="7">
+        <v>0</v>
+      </c>
+      <c r="M26" s="7">
+        <v>2</v>
+      </c>
+      <c r="N26" s="7">
+        <v>3.5</v>
+      </c>
+      <c r="O26" s="7">
+        <v>2.5</v>
+      </c>
+      <c r="P26" s="7">
+        <v>1</v>
+      </c>
+      <c r="Q26" s="7">
+        <v>5</v>
+      </c>
+      <c r="R26" s="7">
+        <v>2</v>
+      </c>
+      <c r="S26" s="7">
+        <v>3</v>
+      </c>
+      <c r="T26" s="7">
+        <v>3</v>
+      </c>
+      <c r="U26" s="7">
+        <v>0</v>
+      </c>
+      <c r="V26" s="7">
+        <v>1.5</v>
+      </c>
+      <c r="W26" s="7">
+        <v>1</v>
+      </c>
+      <c r="X26" s="7">
+        <v>1</v>
+      </c>
+      <c r="Y26" s="7">
+        <v>1</v>
+      </c>
+      <c r="Z26" s="7">
+        <v>1</v>
+      </c>
+      <c r="AA26" s="7">
+        <v>1.5</v>
+      </c>
+      <c r="AB26" s="7">
+        <v>5</v>
+      </c>
+      <c r="AC26" s="7">
+        <v>2.5</v>
+      </c>
+      <c r="AD26" s="7">
+        <v>0</v>
+      </c>
+      <c r="AE26" s="7">
+        <v>0.5</v>
+      </c>
+      <c r="AF26" s="7">
+        <v>2</v>
+      </c>
+      <c r="AG26" s="7">
+        <v>2</v>
+      </c>
+      <c r="AH26" s="7">
+        <v>1</v>
+      </c>
+      <c r="AI26" s="7">
+        <v>0</v>
+      </c>
+      <c r="AJ26" s="7">
+        <v>1.5</v>
+      </c>
+      <c r="AK26" s="7">
+        <v>2</v>
+      </c>
+      <c r="AL26" s="7">
+        <v>3</v>
+      </c>
+      <c r="AM26" s="7">
+        <v>3.5</v>
+      </c>
+      <c r="AN26" s="7">
+        <v>1.5</v>
+      </c>
+      <c r="AO26" s="7">
+        <v>0</v>
+      </c>
+      <c r="AP26" s="7">
+        <v>1</v>
+      </c>
+      <c r="AQ26" s="7">
+        <v>1.5</v>
+      </c>
+      <c r="AR26" s="7">
+        <v>1.5</v>
+      </c>
+      <c r="AS26" s="7">
+        <v>0</v>
+      </c>
+      <c r="AT26" s="7">
+        <v>0</v>
+      </c>
+      <c r="AU26" s="7">
+        <v>2.5</v>
+      </c>
+      <c r="AV26" s="7">
+        <v>0.5</v>
+      </c>
+      <c r="AW26" s="7">
+        <v>2.5</v>
+      </c>
+      <c r="AX26" s="7">
+        <v>0</v>
+      </c>
+      <c r="AY26" s="28">
+        <v>2</v>
+      </c>
       <c r="AZ26" s="28"/>
       <c r="BA26" s="1">
         <f t="shared" si="7"/>
-        <v>0</v>
+        <v>72</v>
       </c>
       <c r="BB26" s="1">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>7200</v>
       </c>
       <c r="BC26" s="1">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>-72</v>
       </c>
       <c r="BD26" s="1">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>-7200</v>
       </c>
     </row>
     <row r="27" spans="1:56">
@@ -5213,19 +5301,19 @@
       </c>
       <c r="H32" s="4">
         <f t="shared" ref="H32:AW32" si="8">SUM(H2:H31)</f>
-        <v>11.5</v>
+        <v>12</v>
       </c>
       <c r="I32" s="4">
         <f t="shared" si="8"/>
-        <v>74.5</v>
+        <v>77.5</v>
       </c>
       <c r="J32" s="4">
         <f t="shared" si="8"/>
-        <v>36</v>
+        <v>37.5</v>
       </c>
       <c r="K32" s="4">
         <f t="shared" si="8"/>
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="L32" s="4">
         <f t="shared" si="8"/>
@@ -5233,35 +5321,35 @@
       </c>
       <c r="M32" s="4">
         <f t="shared" si="8"/>
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="N32" s="4">
         <f t="shared" si="8"/>
-        <v>11.5</v>
+        <v>15</v>
       </c>
       <c r="O32" s="4">
         <f t="shared" si="8"/>
-        <v>55</v>
+        <v>57.5</v>
       </c>
       <c r="P32" s="4">
         <f t="shared" si="8"/>
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="Q32" s="4">
         <f t="shared" si="8"/>
-        <v>120</v>
+        <v>125</v>
       </c>
       <c r="R32" s="4">
         <f t="shared" si="8"/>
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="S32" s="4">
         <f t="shared" si="8"/>
-        <v>73</v>
+        <v>76</v>
       </c>
       <c r="T32" s="4">
         <f t="shared" si="8"/>
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="U32" s="4">
         <f t="shared" si="8"/>
@@ -5269,35 +5357,35 @@
       </c>
       <c r="V32" s="4">
         <f t="shared" si="8"/>
-        <v>36</v>
+        <v>37.5</v>
       </c>
       <c r="W32" s="4">
         <f t="shared" si="8"/>
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="X32" s="4">
         <f t="shared" si="8"/>
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="Y32" s="4">
         <f t="shared" si="8"/>
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="Z32" s="4">
         <f t="shared" si="8"/>
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="AA32" s="4">
         <f t="shared" si="8"/>
-        <v>31</v>
+        <v>32.5</v>
       </c>
       <c r="AB32" s="4">
         <f t="shared" si="8"/>
-        <v>120</v>
+        <v>125</v>
       </c>
       <c r="AC32" s="4">
         <f t="shared" si="8"/>
-        <v>60</v>
+        <v>62.5</v>
       </c>
       <c r="AD32" s="4">
         <f t="shared" si="8"/>
@@ -5305,19 +5393,19 @@
       </c>
       <c r="AE32" s="4">
         <f t="shared" si="8"/>
-        <v>12</v>
+        <v>12.5</v>
       </c>
       <c r="AF32" s="4">
         <f t="shared" si="8"/>
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="AG32" s="4">
         <f t="shared" si="8"/>
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="AH32" s="4">
         <f t="shared" si="8"/>
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="AI32" s="4">
         <f t="shared" si="8"/>
@@ -5325,23 +5413,23 @@
       </c>
       <c r="AJ32" s="4">
         <f t="shared" si="8"/>
-        <v>36</v>
+        <v>37.5</v>
       </c>
       <c r="AK32" s="4">
         <f t="shared" si="8"/>
-        <v>83.5</v>
+        <v>85.5</v>
       </c>
       <c r="AL32" s="4">
         <f t="shared" si="8"/>
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="AM32" s="4">
         <f t="shared" si="8"/>
-        <v>84</v>
+        <v>87.5</v>
       </c>
       <c r="AN32" s="4">
         <f t="shared" si="8"/>
-        <v>36</v>
+        <v>37.5</v>
       </c>
       <c r="AO32" s="4">
         <f t="shared" si="8"/>
@@ -5349,15 +5437,15 @@
       </c>
       <c r="AP32" s="4">
         <f t="shared" si="8"/>
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="AQ32" s="4">
         <f t="shared" si="8"/>
-        <v>46.5</v>
+        <v>48</v>
       </c>
       <c r="AR32" s="4">
         <f t="shared" si="8"/>
-        <v>36</v>
+        <v>37.5</v>
       </c>
       <c r="AS32" s="4">
         <f t="shared" si="8"/>
@@ -5369,19 +5457,19 @@
       </c>
       <c r="AU32" s="4">
         <f t="shared" si="8"/>
-        <v>55</v>
+        <v>57.5</v>
       </c>
       <c r="AV32" s="4">
         <f t="shared" si="8"/>
-        <v>9.5</v>
+        <v>10</v>
       </c>
       <c r="AW32" s="4">
         <f t="shared" si="8"/>
-        <v>58</v>
+        <v>60.5</v>
       </c>
       <c r="AY32" s="4">
         <f>SUM(AY2:AY31)</f>
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="AZ32" s="4">
         <f>SUM(AZ2:AZ31)</f>
@@ -5389,19 +5477,19 @@
       </c>
       <c r="BA32" s="4">
         <f>SUM(BA2:BA31)</f>
-        <v>1775</v>
+        <v>1847</v>
       </c>
       <c r="BB32" s="4">
         <f>SUM(BB2:BB31)</f>
-        <v>177500</v>
+        <v>184700</v>
       </c>
       <c r="BC32" s="4">
         <f>SUM(BC2:BC29)</f>
-        <v>-1672.5</v>
+        <v>-1744.5</v>
       </c>
       <c r="BD32" s="4">
         <f>SUM(BD2:BD29)</f>
-        <v>-177397.5</v>
+        <v>-184597.5</v>
       </c>
     </row>
     <row r="33" spans="1:53" s="10" customFormat="1">
@@ -5410,19 +5498,19 @@
       </c>
       <c r="H33" s="10">
         <f>H32*90</f>
-        <v>1035</v>
+        <v>1080</v>
       </c>
       <c r="I33" s="10">
         <f>I32*120</f>
-        <v>8940</v>
+        <v>9300</v>
       </c>
       <c r="J33" s="10">
         <f>J32*120</f>
-        <v>4320</v>
+        <v>4500</v>
       </c>
       <c r="K33" s="10">
         <f>K32*110</f>
-        <v>5280</v>
+        <v>5500</v>
       </c>
       <c r="L33" s="10">
         <f>L32*120</f>
@@ -5430,35 +5518,35 @@
       </c>
       <c r="M33" s="10">
         <f>M32*100</f>
-        <v>1600</v>
+        <v>1800</v>
       </c>
       <c r="N33" s="10">
         <f>N32*100</f>
-        <v>1150</v>
+        <v>1500</v>
       </c>
       <c r="O33" s="10">
         <f>O32*120</f>
-        <v>6600</v>
+        <v>6900</v>
       </c>
       <c r="P33" s="10">
         <f>P32*100</f>
-        <v>2400</v>
+        <v>2500</v>
       </c>
       <c r="Q33" s="10">
         <f>Q32*120</f>
-        <v>14400</v>
+        <v>15000</v>
       </c>
       <c r="R33" s="10">
         <f t="shared" ref="R33:U33" si="9">R32*120</f>
-        <v>5760</v>
+        <v>6000</v>
       </c>
       <c r="S33" s="10">
         <f>S32*120</f>
-        <v>8760</v>
+        <v>9120</v>
       </c>
       <c r="T33" s="10">
         <f>T32*120</f>
-        <v>8640</v>
+        <v>9000</v>
       </c>
       <c r="U33" s="10">
         <f t="shared" si="9"/>
@@ -5466,35 +5554,35 @@
       </c>
       <c r="V33" s="10">
         <f>V32*110</f>
-        <v>3960</v>
+        <v>4125</v>
       </c>
       <c r="W33" s="10">
         <f>W32*120</f>
-        <v>2880</v>
+        <v>3000</v>
       </c>
       <c r="X33" s="10">
         <f>X32*110</f>
-        <v>2640</v>
+        <v>2750</v>
       </c>
       <c r="Y33" s="10">
         <f>Y32*100</f>
-        <v>2400</v>
+        <v>2500</v>
       </c>
       <c r="Z33" s="10">
         <f>Z32*100</f>
-        <v>2400</v>
+        <v>2500</v>
       </c>
       <c r="AA33" s="10">
         <f>AA32*110</f>
-        <v>3410</v>
+        <v>3575</v>
       </c>
       <c r="AB33" s="11">
         <f>AB32*120</f>
-        <v>14400</v>
+        <v>15000</v>
       </c>
       <c r="AC33" s="11">
         <f>AC32*100</f>
-        <v>6000</v>
+        <v>6250</v>
       </c>
       <c r="AD33" s="11">
         <f>AD32*100</f>
@@ -5502,19 +5590,19 @@
       </c>
       <c r="AE33" s="11">
         <f>AE32*110</f>
-        <v>1320</v>
+        <v>1375</v>
       </c>
       <c r="AF33" s="11">
         <f>AF32*110</f>
-        <v>5610</v>
+        <v>5830</v>
       </c>
       <c r="AG33" s="12">
         <f>AG32*110</f>
-        <v>5280</v>
+        <v>5500</v>
       </c>
       <c r="AH33" s="11">
         <f>AH32*110</f>
-        <v>2640</v>
+        <v>2750</v>
       </c>
       <c r="AI33" s="11">
         <f>AI32*120</f>
@@ -5522,23 +5610,23 @@
       </c>
       <c r="AJ33" s="11">
         <f>AJ32*120</f>
-        <v>4320</v>
+        <v>4500</v>
       </c>
       <c r="AK33" s="11">
         <f>AK32*120</f>
-        <v>10020</v>
+        <v>10260</v>
       </c>
       <c r="AL33" s="11">
         <f>AL32*120</f>
-        <v>8280</v>
+        <v>8640</v>
       </c>
       <c r="AM33" s="11">
         <f t="shared" ref="AM33" si="10">AM32*120</f>
-        <v>10080</v>
+        <v>10500</v>
       </c>
       <c r="AN33" s="11">
         <f>AN32*120</f>
-        <v>4320</v>
+        <v>4500</v>
       </c>
       <c r="AO33" s="11">
         <f>AO32*120</f>
@@ -5546,15 +5634,15 @@
       </c>
       <c r="AP33" s="11">
         <f>AP32*120</f>
-        <v>2880</v>
+        <v>3000</v>
       </c>
       <c r="AQ33" s="11">
         <f>AQ32*120</f>
-        <v>5580</v>
+        <v>5760</v>
       </c>
       <c r="AR33" s="11">
         <f>AR32*110</f>
-        <v>3960</v>
+        <v>4125</v>
       </c>
       <c r="AS33" s="11">
         <f>AS32*120</f>
@@ -5566,20 +5654,20 @@
       </c>
       <c r="AU33" s="11">
         <f>AU32*120</f>
-        <v>6600</v>
+        <v>6900</v>
       </c>
       <c r="AV33" s="11">
         <f>AV32*120</f>
-        <v>1140</v>
+        <v>1200</v>
       </c>
       <c r="AW33" s="11">
         <f>AW32*120</f>
-        <v>6960</v>
+        <v>7260</v>
       </c>
       <c r="AX33" s="11"/>
       <c r="AY33" s="11">
         <f>AY32*120</f>
-        <v>4080</v>
+        <v>4320</v>
       </c>
       <c r="AZ33" s="11">
         <f>AZ32*110</f>
@@ -5587,7 +5675,7 @@
       </c>
       <c r="BA33" s="9">
         <f>SUM(H33:AZ33)</f>
-        <v>205675</v>
+        <v>213950</v>
       </c>
     </row>
     <row r="34" spans="1:53" s="13" customFormat="1">
@@ -6021,19 +6109,19 @@
       </c>
       <c r="H37" s="17">
         <f>(H36+H35)-(H33+H34)</f>
-        <v>-1035</v>
+        <v>-1080</v>
       </c>
       <c r="I37" s="17">
         <f>(I36+I35)-(I33+I34)</f>
-        <v>-8940</v>
+        <v>-9300</v>
       </c>
       <c r="J37" s="17">
         <f t="shared" ref="J37:BA37" si="11">(J36+J35)-(J33+J34)</f>
-        <v>-4320</v>
+        <v>-4500</v>
       </c>
       <c r="K37" s="17">
         <f t="shared" si="11"/>
-        <v>-5280</v>
+        <v>-5500</v>
       </c>
       <c r="L37" s="17">
         <f t="shared" si="11"/>
@@ -6041,35 +6129,35 @@
       </c>
       <c r="M37" s="17">
         <f t="shared" si="11"/>
-        <v>-1600</v>
+        <v>-1800</v>
       </c>
       <c r="N37" s="17">
         <f t="shared" si="11"/>
-        <v>-1150</v>
+        <v>-1500</v>
       </c>
       <c r="O37" s="17">
         <f t="shared" si="11"/>
-        <v>-6600</v>
+        <v>-6900</v>
       </c>
       <c r="P37" s="17">
         <f t="shared" si="11"/>
-        <v>600</v>
+        <v>500</v>
       </c>
       <c r="Q37" s="17">
         <f t="shared" si="11"/>
-        <v>-14400</v>
+        <v>-15000</v>
       </c>
       <c r="R37" s="17">
         <f t="shared" si="11"/>
-        <v>-5760</v>
+        <v>-6000</v>
       </c>
       <c r="S37" s="17">
         <f t="shared" si="11"/>
-        <v>-8760</v>
+        <v>-9120</v>
       </c>
       <c r="T37" s="17">
         <f t="shared" si="11"/>
-        <v>-8640</v>
+        <v>-9000</v>
       </c>
       <c r="U37" s="17">
         <f t="shared" si="11"/>
@@ -6077,35 +6165,35 @@
       </c>
       <c r="V37" s="17">
         <f t="shared" si="11"/>
-        <v>-3960</v>
+        <v>-4125</v>
       </c>
       <c r="W37" s="17">
         <f t="shared" si="11"/>
-        <v>-2880</v>
+        <v>-3000</v>
       </c>
       <c r="X37" s="17">
         <f t="shared" si="11"/>
-        <v>-2640</v>
+        <v>-2750</v>
       </c>
       <c r="Y37" s="17">
         <f t="shared" si="11"/>
-        <v>-2400</v>
+        <v>-2500</v>
       </c>
       <c r="Z37" s="17">
         <f t="shared" si="11"/>
-        <v>-2400</v>
+        <v>-2500</v>
       </c>
       <c r="AA37" s="17">
         <f t="shared" si="11"/>
-        <v>-3410</v>
+        <v>-3575</v>
       </c>
       <c r="AB37" s="17">
         <f t="shared" si="11"/>
-        <v>-14400</v>
+        <v>-15000</v>
       </c>
       <c r="AC37" s="17">
         <f t="shared" si="11"/>
-        <v>-6000</v>
+        <v>-6250</v>
       </c>
       <c r="AD37" s="17">
         <f t="shared" si="11"/>
@@ -6113,19 +6201,19 @@
       </c>
       <c r="AE37" s="17">
         <f t="shared" si="11"/>
-        <v>-1320</v>
+        <v>-1375</v>
       </c>
       <c r="AF37" s="17">
         <f t="shared" si="11"/>
-        <v>-5610</v>
+        <v>-5830</v>
       </c>
       <c r="AG37" s="17">
         <f t="shared" si="11"/>
-        <v>-5280</v>
+        <v>-5500</v>
       </c>
       <c r="AH37" s="17">
         <f t="shared" si="11"/>
-        <v>-2640</v>
+        <v>-2750</v>
       </c>
       <c r="AI37" s="17">
         <f t="shared" si="11"/>
@@ -6133,23 +6221,23 @@
       </c>
       <c r="AJ37" s="17">
         <f t="shared" si="11"/>
-        <v>-14385</v>
+        <v>-14565</v>
       </c>
       <c r="AK37" s="17">
         <f t="shared" si="11"/>
-        <v>-10020</v>
+        <v>-10260</v>
       </c>
       <c r="AL37" s="17">
         <f t="shared" si="11"/>
-        <v>-8280</v>
+        <v>-8640</v>
       </c>
       <c r="AM37" s="17">
         <f t="shared" si="11"/>
-        <v>-10080</v>
+        <v>-10500</v>
       </c>
       <c r="AN37" s="17">
         <f t="shared" si="11"/>
-        <v>-4320</v>
+        <v>-4500</v>
       </c>
       <c r="AO37" s="17">
         <f t="shared" si="11"/>
@@ -6157,15 +6245,15 @@
       </c>
       <c r="AP37" s="17">
         <f t="shared" si="11"/>
-        <v>-2880</v>
+        <v>-3000</v>
       </c>
       <c r="AQ37" s="17">
         <f t="shared" si="11"/>
-        <v>-5580</v>
+        <v>-5760</v>
       </c>
       <c r="AR37" s="17">
         <f t="shared" si="11"/>
-        <v>-3960</v>
+        <v>-4125</v>
       </c>
       <c r="AS37" s="17">
         <f t="shared" si="11"/>
@@ -6177,19 +6265,19 @@
       </c>
       <c r="AU37" s="17">
         <f t="shared" si="11"/>
-        <v>-6600</v>
+        <v>-6900</v>
       </c>
       <c r="AV37" s="17">
         <f t="shared" si="11"/>
-        <v>-1140</v>
+        <v>-1200</v>
       </c>
       <c r="AW37" s="17">
         <f t="shared" si="11"/>
-        <v>-6960</v>
+        <v>-7260</v>
       </c>
       <c r="AY37" s="17">
         <f>(AY36+AY35)-(AY33+AY34)</f>
-        <v>-4080</v>
+        <v>-4320</v>
       </c>
       <c r="AZ37" s="17">
         <f t="shared" si="11"/>
@@ -6197,7 +6285,7 @@
       </c>
       <c r="BA37" s="18">
         <f t="shared" si="11"/>
-        <v>-215740</v>
+        <v>-224015</v>
       </c>
     </row>
     <row r="39" spans="1:53">

</xml_diff>

<commit_message>
sheel update nov 30, 2021
</commit_message>
<xml_diff>
--- a/2021/november,  2021.xlsx
+++ b/2021/november,  2021.xlsx
@@ -100,9 +100,6 @@
     <t>abdulRashid</t>
   </si>
   <si>
-    <t>apya</t>
-  </si>
-  <si>
     <t>qari ramzan sb</t>
   </si>
   <si>
@@ -188,6 +185,9 @@
   </si>
   <si>
     <t>shafqat</t>
+  </si>
+  <si>
+    <t>zahid ur Rehman</t>
   </si>
 </sst>
 </file>
@@ -338,7 +338,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
@@ -371,7 +371,6 @@
     <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Calculation" xfId="1" builtinId="22"/>
@@ -669,8 +668,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:BD39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AR1" workbookViewId="0">
-      <selection activeCell="BB26" sqref="BB26"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H27" sqref="H27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -697,19 +696,19 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C1" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="E1" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="F1" s="2" t="s">
         <v>43</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>44</v>
       </c>
       <c r="G1" s="2" t="s">
         <v>3</v>
@@ -730,22 +729,22 @@
         <v>6</v>
       </c>
       <c r="M1" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="N1" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="N1" s="2" t="s">
-        <v>57</v>
-      </c>
       <c r="O1" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="P1" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="Q1" s="2" t="s">
         <v>9</v>
       </c>
       <c r="R1" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="S1" s="2" t="s">
         <v>10</v>
@@ -778,76 +777,76 @@
         <v>19</v>
       </c>
       <c r="AC1" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="AD1" s="2" t="s">
-        <v>28</v>
+        <v>57</v>
       </c>
       <c r="AE1" s="2" t="s">
         <v>25</v>
       </c>
       <c r="AF1" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="AG1" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="AH1" s="2" t="s">
         <v>24</v>
       </c>
       <c r="AI1" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="AJ1" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="AJ1" s="2" t="s">
+      <c r="AK1" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="AL1" s="2" t="s">
         <v>31</v>
-      </c>
-      <c r="AK1" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="AL1" s="2" t="s">
-        <v>32</v>
       </c>
       <c r="AM1" s="2" t="s">
         <v>21</v>
       </c>
       <c r="AN1" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="AO1" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="AP1" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="AQ1" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="AO1" s="2" t="s">
+      <c r="AR1" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="AP1" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="AQ1" s="2" t="s">
+      <c r="AS1" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="AT1" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="AR1" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="AS1" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="AT1" s="2" t="s">
+      <c r="AU1" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="AU1" s="2" t="s">
-        <v>36</v>
-      </c>
       <c r="AV1" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="AW1" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="AX1" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="AY1" s="2" t="s">
         <v>11</v>
       </c>
       <c r="AZ1" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="BA1" s="2" t="s">
         <v>7</v>
@@ -892,7 +891,7 @@
         <v>2</v>
       </c>
       <c r="L2" s="7">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="M2" s="7">
         <v>0</v>
@@ -1014,19 +1013,19 @@
       <c r="AZ2" s="7"/>
       <c r="BA2" s="6">
         <f t="shared" ref="BA2:BA9" si="0">SUM(H2:AZ2)</f>
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="BB2" s="6">
         <f>BA2*100</f>
-        <v>6600</v>
+        <v>6800</v>
       </c>
       <c r="BC2" s="6">
         <f t="shared" ref="BC2:BC31" si="1">G2-BA2</f>
-        <v>-50</v>
+        <v>-52</v>
       </c>
       <c r="BD2" s="29">
         <f t="shared" ref="BD2:BD31" si="2">G2-BB2</f>
-        <v>-6584</v>
+        <v>-6784</v>
       </c>
     </row>
     <row r="3" spans="1:56" s="29" customFormat="1">
@@ -4621,7 +4620,7 @@
         <v>2</v>
       </c>
       <c r="L25" s="7">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="M25" s="7">
         <v>2</v>
@@ -4741,19 +4740,19 @@
       <c r="AZ25" s="28"/>
       <c r="BA25" s="1">
         <f t="shared" si="7"/>
-        <v>73.5</v>
+        <v>75.5</v>
       </c>
       <c r="BB25" s="1">
         <f t="shared" si="3"/>
-        <v>7350</v>
+        <v>7550</v>
       </c>
       <c r="BC25" s="1">
         <f t="shared" si="1"/>
-        <v>-73.5</v>
+        <v>-75.5</v>
       </c>
       <c r="BD25" s="1">
         <f t="shared" si="2"/>
-        <v>-7350</v>
+        <v>-7550</v>
       </c>
     </row>
     <row r="26" spans="1:56">
@@ -4782,7 +4781,7 @@
         <v>2</v>
       </c>
       <c r="L26" s="7">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="M26" s="7">
         <v>2</v>
@@ -4904,19 +4903,19 @@
       <c r="AZ26" s="28"/>
       <c r="BA26" s="1">
         <f t="shared" si="7"/>
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="BB26" s="1">
         <f t="shared" si="3"/>
-        <v>7200</v>
+        <v>7400</v>
       </c>
       <c r="BC26" s="1">
         <f t="shared" si="1"/>
-        <v>-72</v>
+        <v>-74</v>
       </c>
       <c r="BD26" s="1">
         <f t="shared" si="2"/>
-        <v>-7200</v>
+        <v>-7400</v>
       </c>
     </row>
     <row r="27" spans="1:56">
@@ -4932,66 +4931,152 @@
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="H27" s="7"/>
-      <c r="I27" s="7"/>
-      <c r="J27" s="7"/>
-      <c r="K27" s="7"/>
-      <c r="L27" s="7"/>
-      <c r="M27" s="7"/>
-      <c r="N27" s="7"/>
-      <c r="O27" s="7"/>
-      <c r="P27" s="7"/>
-      <c r="Q27" s="7"/>
-      <c r="R27" s="7"/>
-      <c r="S27" s="7"/>
-      <c r="T27" s="7"/>
-      <c r="U27" s="7"/>
-      <c r="V27" s="7"/>
-      <c r="W27" s="7"/>
-      <c r="X27" s="7"/>
-      <c r="Y27" s="7"/>
-      <c r="Z27" s="7"/>
-      <c r="AA27" s="7"/>
-      <c r="AB27" s="7"/>
-      <c r="AC27" s="7"/>
-      <c r="AD27" s="7"/>
-      <c r="AE27" s="7"/>
-      <c r="AF27" s="7"/>
-      <c r="AG27" s="7"/>
-      <c r="AH27" s="7"/>
-      <c r="AI27" s="7"/>
-      <c r="AJ27" s="7"/>
-      <c r="AK27" s="7"/>
-      <c r="AL27" s="7"/>
-      <c r="AM27" s="7"/>
-      <c r="AN27" s="7"/>
-      <c r="AO27" s="7"/>
-      <c r="AP27" s="7"/>
-      <c r="AQ27" s="7"/>
-      <c r="AR27" s="7"/>
-      <c r="AS27" s="7"/>
-      <c r="AT27" s="7"/>
-      <c r="AU27" s="7"/>
-      <c r="AV27" s="7"/>
-      <c r="AW27" s="7"/>
-      <c r="AX27" s="7"/>
+      <c r="H27" s="7">
+        <v>0.5</v>
+      </c>
+      <c r="I27" s="7">
+        <v>3</v>
+      </c>
+      <c r="J27" s="7">
+        <v>1.5</v>
+      </c>
+      <c r="K27" s="7">
+        <v>2</v>
+      </c>
+      <c r="L27" s="7">
+        <v>2</v>
+      </c>
+      <c r="M27" s="7">
+        <v>2</v>
+      </c>
+      <c r="N27" s="7">
+        <v>3.5</v>
+      </c>
+      <c r="O27" s="7">
+        <v>2.5</v>
+      </c>
+      <c r="P27" s="7">
+        <v>1</v>
+      </c>
+      <c r="Q27" s="7">
+        <v>5</v>
+      </c>
+      <c r="R27" s="7">
+        <v>2</v>
+      </c>
+      <c r="S27" s="7">
+        <v>3</v>
+      </c>
+      <c r="T27" s="7">
+        <v>3</v>
+      </c>
+      <c r="U27" s="7">
+        <v>0</v>
+      </c>
+      <c r="V27" s="7">
+        <v>1.5</v>
+      </c>
+      <c r="W27" s="7">
+        <v>1</v>
+      </c>
+      <c r="X27" s="7">
+        <v>1</v>
+      </c>
+      <c r="Y27" s="7">
+        <v>1</v>
+      </c>
+      <c r="Z27" s="7">
+        <v>1</v>
+      </c>
+      <c r="AA27" s="7">
+        <v>1.5</v>
+      </c>
+      <c r="AB27" s="7">
+        <v>5</v>
+      </c>
+      <c r="AC27" s="7">
+        <v>2.5</v>
+      </c>
+      <c r="AD27" s="7">
+        <v>0</v>
+      </c>
+      <c r="AE27" s="7">
+        <v>0.5</v>
+      </c>
+      <c r="AF27" s="7">
+        <v>2</v>
+      </c>
+      <c r="AG27" s="7">
+        <v>2</v>
+      </c>
+      <c r="AH27" s="7">
+        <v>1</v>
+      </c>
+      <c r="AI27" s="7">
+        <v>0</v>
+      </c>
+      <c r="AJ27" s="7">
+        <v>1.5</v>
+      </c>
+      <c r="AK27" s="7">
+        <v>2</v>
+      </c>
+      <c r="AL27" s="7">
+        <v>3</v>
+      </c>
+      <c r="AM27" s="7">
+        <v>3.5</v>
+      </c>
+      <c r="AN27" s="7">
+        <v>1.5</v>
+      </c>
+      <c r="AO27" s="7">
+        <v>0</v>
+      </c>
+      <c r="AP27" s="7">
+        <v>1</v>
+      </c>
+      <c r="AQ27" s="7">
+        <v>1.5</v>
+      </c>
+      <c r="AR27" s="7">
+        <v>1.5</v>
+      </c>
+      <c r="AS27" s="7">
+        <v>2</v>
+      </c>
+      <c r="AT27" s="7">
+        <v>0</v>
+      </c>
+      <c r="AU27" s="7">
+        <v>2.5</v>
+      </c>
+      <c r="AV27" s="7">
+        <v>0.5</v>
+      </c>
+      <c r="AW27" s="7">
+        <v>2.5</v>
+      </c>
+      <c r="AX27" s="7">
+        <v>0</v>
+      </c>
       <c r="AY27" s="28"/>
       <c r="AZ27" s="28"/>
       <c r="BA27" s="1">
         <f t="shared" si="7"/>
-        <v>0</v>
+        <v>74</v>
       </c>
       <c r="BB27" s="1">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>7400</v>
       </c>
       <c r="BC27" s="1">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>-74</v>
       </c>
       <c r="BD27" s="1">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>-7400</v>
       </c>
     </row>
     <row r="28" spans="1:56">
@@ -5007,66 +5092,152 @@
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="H28" s="7"/>
-      <c r="I28" s="7"/>
-      <c r="J28" s="7"/>
-      <c r="K28" s="7"/>
-      <c r="L28" s="7"/>
-      <c r="M28" s="7"/>
-      <c r="N28" s="7"/>
-      <c r="O28" s="7"/>
-      <c r="P28" s="7"/>
-      <c r="Q28" s="7"/>
-      <c r="R28" s="7"/>
-      <c r="S28" s="7"/>
-      <c r="T28" s="7"/>
-      <c r="U28" s="7"/>
-      <c r="V28" s="7"/>
-      <c r="W28" s="7"/>
-      <c r="X28" s="7"/>
-      <c r="Y28" s="7"/>
-      <c r="Z28" s="7"/>
-      <c r="AA28" s="7"/>
-      <c r="AB28" s="7"/>
-      <c r="AC28" s="7"/>
-      <c r="AD28" s="7"/>
-      <c r="AE28" s="7"/>
-      <c r="AF28" s="7"/>
-      <c r="AG28" s="7"/>
-      <c r="AH28" s="7"/>
-      <c r="AI28" s="7"/>
-      <c r="AJ28" s="7"/>
-      <c r="AK28" s="7"/>
-      <c r="AL28" s="7"/>
-      <c r="AM28" s="7"/>
-      <c r="AN28" s="7"/>
-      <c r="AO28" s="7"/>
-      <c r="AP28" s="7"/>
-      <c r="AQ28" s="7"/>
-      <c r="AR28" s="7"/>
-      <c r="AS28" s="7"/>
-      <c r="AT28" s="7"/>
-      <c r="AU28" s="7"/>
-      <c r="AV28" s="7"/>
-      <c r="AW28" s="7"/>
-      <c r="AX28" s="7"/>
+      <c r="H28" s="7">
+        <v>0.5</v>
+      </c>
+      <c r="I28" s="7">
+        <v>3</v>
+      </c>
+      <c r="J28" s="7">
+        <v>1.5</v>
+      </c>
+      <c r="K28" s="7">
+        <v>2</v>
+      </c>
+      <c r="L28" s="7">
+        <v>2</v>
+      </c>
+      <c r="M28" s="7">
+        <v>2</v>
+      </c>
+      <c r="N28" s="7">
+        <v>3.5</v>
+      </c>
+      <c r="O28" s="7">
+        <v>2.5</v>
+      </c>
+      <c r="P28" s="7">
+        <v>1</v>
+      </c>
+      <c r="Q28" s="7">
+        <v>5</v>
+      </c>
+      <c r="R28" s="7">
+        <v>2</v>
+      </c>
+      <c r="S28" s="7">
+        <v>3</v>
+      </c>
+      <c r="T28" s="7">
+        <v>3</v>
+      </c>
+      <c r="U28" s="7">
+        <v>0</v>
+      </c>
+      <c r="V28" s="7">
+        <v>1.5</v>
+      </c>
+      <c r="W28" s="7">
+        <v>1</v>
+      </c>
+      <c r="X28" s="7">
+        <v>1</v>
+      </c>
+      <c r="Y28" s="7">
+        <v>1</v>
+      </c>
+      <c r="Z28" s="7">
+        <v>1</v>
+      </c>
+      <c r="AA28" s="7">
+        <v>1.5</v>
+      </c>
+      <c r="AB28" s="7">
+        <v>5</v>
+      </c>
+      <c r="AC28" s="7">
+        <v>2.5</v>
+      </c>
+      <c r="AD28" s="7">
+        <v>0</v>
+      </c>
+      <c r="AE28" s="7">
+        <v>0.5</v>
+      </c>
+      <c r="AF28" s="7">
+        <v>2</v>
+      </c>
+      <c r="AG28" s="7">
+        <v>2</v>
+      </c>
+      <c r="AH28" s="7">
+        <v>1</v>
+      </c>
+      <c r="AI28" s="7">
+        <v>0</v>
+      </c>
+      <c r="AJ28" s="7">
+        <v>1.5</v>
+      </c>
+      <c r="AK28" s="7">
+        <v>2</v>
+      </c>
+      <c r="AL28" s="7">
+        <v>3</v>
+      </c>
+      <c r="AM28" s="7">
+        <v>3.5</v>
+      </c>
+      <c r="AN28" s="7">
+        <v>1.5</v>
+      </c>
+      <c r="AO28" s="7">
+        <v>0</v>
+      </c>
+      <c r="AP28" s="7">
+        <v>1</v>
+      </c>
+      <c r="AQ28" s="7">
+        <v>1.5</v>
+      </c>
+      <c r="AR28" s="7">
+        <v>1.5</v>
+      </c>
+      <c r="AS28" s="7">
+        <v>0</v>
+      </c>
+      <c r="AT28" s="7">
+        <v>0</v>
+      </c>
+      <c r="AU28" s="7">
+        <v>2.5</v>
+      </c>
+      <c r="AV28" s="7">
+        <v>0.5</v>
+      </c>
+      <c r="AW28" s="7">
+        <v>2.5</v>
+      </c>
+      <c r="AX28" s="7">
+        <v>0</v>
+      </c>
       <c r="AY28" s="28"/>
       <c r="AZ28" s="28"/>
       <c r="BA28" s="1">
         <f t="shared" si="7"/>
-        <v>0</v>
+        <v>72</v>
       </c>
       <c r="BB28" s="1">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>7200</v>
       </c>
       <c r="BC28" s="1">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>-72</v>
       </c>
       <c r="BD28" s="1">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>-7200</v>
       </c>
     </row>
     <row r="29" spans="1:56">
@@ -5082,66 +5253,152 @@
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="H29" s="7"/>
-      <c r="I29" s="7"/>
-      <c r="J29" s="7"/>
-      <c r="K29" s="7"/>
-      <c r="L29" s="7"/>
-      <c r="M29" s="7"/>
-      <c r="N29" s="7"/>
-      <c r="O29" s="7"/>
-      <c r="P29" s="7"/>
-      <c r="Q29" s="7"/>
-      <c r="R29" s="7"/>
-      <c r="S29" s="7"/>
-      <c r="T29" s="7"/>
-      <c r="U29" s="7"/>
-      <c r="V29" s="7"/>
-      <c r="W29" s="7"/>
-      <c r="X29" s="7"/>
-      <c r="Y29" s="7"/>
-      <c r="Z29" s="7"/>
-      <c r="AA29" s="7"/>
-      <c r="AB29" s="7"/>
-      <c r="AC29" s="7"/>
-      <c r="AD29" s="7"/>
-      <c r="AE29" s="7"/>
-      <c r="AF29" s="7"/>
-      <c r="AG29" s="7"/>
-      <c r="AH29" s="32"/>
-      <c r="AI29" s="7"/>
-      <c r="AJ29" s="7"/>
-      <c r="AK29" s="7"/>
-      <c r="AL29" s="7"/>
-      <c r="AM29" s="7"/>
-      <c r="AN29" s="7"/>
-      <c r="AO29" s="7"/>
-      <c r="AP29" s="7"/>
-      <c r="AQ29" s="7"/>
-      <c r="AR29" s="7"/>
-      <c r="AS29" s="7"/>
-      <c r="AT29" s="7"/>
-      <c r="AU29" s="7"/>
-      <c r="AV29" s="7"/>
-      <c r="AW29" s="7"/>
-      <c r="AX29" s="7"/>
+      <c r="H29" s="7">
+        <v>0.5</v>
+      </c>
+      <c r="I29" s="7">
+        <v>3</v>
+      </c>
+      <c r="J29" s="7">
+        <v>1.5</v>
+      </c>
+      <c r="K29" s="7">
+        <v>2</v>
+      </c>
+      <c r="L29" s="7">
+        <v>2</v>
+      </c>
+      <c r="M29" s="7">
+        <v>2</v>
+      </c>
+      <c r="N29" s="7">
+        <v>3.5</v>
+      </c>
+      <c r="O29" s="7">
+        <v>2.5</v>
+      </c>
+      <c r="P29" s="7">
+        <v>1</v>
+      </c>
+      <c r="Q29" s="7">
+        <v>5</v>
+      </c>
+      <c r="R29" s="7">
+        <v>2</v>
+      </c>
+      <c r="S29" s="7">
+        <v>3</v>
+      </c>
+      <c r="T29" s="7">
+        <v>3</v>
+      </c>
+      <c r="U29" s="7">
+        <v>0</v>
+      </c>
+      <c r="V29" s="7">
+        <v>1.5</v>
+      </c>
+      <c r="W29" s="7">
+        <v>1</v>
+      </c>
+      <c r="X29" s="7">
+        <v>1</v>
+      </c>
+      <c r="Y29" s="7">
+        <v>1</v>
+      </c>
+      <c r="Z29" s="7">
+        <v>1</v>
+      </c>
+      <c r="AA29" s="7">
+        <v>1.5</v>
+      </c>
+      <c r="AB29" s="7">
+        <v>5</v>
+      </c>
+      <c r="AC29" s="7">
+        <v>2.5</v>
+      </c>
+      <c r="AD29" s="7">
+        <v>0</v>
+      </c>
+      <c r="AE29" s="7">
+        <v>0.5</v>
+      </c>
+      <c r="AF29" s="7">
+        <v>2</v>
+      </c>
+      <c r="AG29" s="7">
+        <v>2</v>
+      </c>
+      <c r="AH29" s="7">
+        <v>1</v>
+      </c>
+      <c r="AI29" s="7">
+        <v>0</v>
+      </c>
+      <c r="AJ29" s="7">
+        <v>1.5</v>
+      </c>
+      <c r="AK29" s="7">
+        <v>2</v>
+      </c>
+      <c r="AL29" s="7">
+        <v>0</v>
+      </c>
+      <c r="AM29" s="7">
+        <v>3.5</v>
+      </c>
+      <c r="AN29" s="7">
+        <v>1.5</v>
+      </c>
+      <c r="AO29" s="7">
+        <v>0</v>
+      </c>
+      <c r="AP29" s="7">
+        <v>1</v>
+      </c>
+      <c r="AQ29" s="7">
+        <v>1.5</v>
+      </c>
+      <c r="AR29" s="7">
+        <v>1.5</v>
+      </c>
+      <c r="AS29" s="7">
+        <v>0</v>
+      </c>
+      <c r="AT29" s="7">
+        <v>0</v>
+      </c>
+      <c r="AU29" s="7">
+        <v>2.5</v>
+      </c>
+      <c r="AV29" s="7">
+        <v>0.5</v>
+      </c>
+      <c r="AW29" s="7">
+        <v>2.5</v>
+      </c>
+      <c r="AX29" s="7">
+        <v>0</v>
+      </c>
       <c r="AY29" s="28"/>
       <c r="AZ29" s="28"/>
       <c r="BA29" s="1">
         <f t="shared" si="7"/>
-        <v>0</v>
+        <v>69</v>
       </c>
       <c r="BB29" s="1">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>6900</v>
       </c>
       <c r="BC29" s="1">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>-69</v>
       </c>
       <c r="BD29" s="1">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>-6900</v>
       </c>
     </row>
     <row r="30" spans="1:56">
@@ -5157,66 +5414,152 @@
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="H30" s="7"/>
-      <c r="I30" s="7"/>
-      <c r="J30" s="7"/>
-      <c r="K30" s="7"/>
-      <c r="L30" s="7"/>
-      <c r="M30" s="7"/>
-      <c r="N30" s="7"/>
-      <c r="O30" s="7"/>
-      <c r="P30" s="7"/>
-      <c r="Q30" s="7"/>
-      <c r="R30" s="7"/>
-      <c r="S30" s="7"/>
-      <c r="T30" s="7"/>
-      <c r="U30" s="7"/>
-      <c r="V30" s="7"/>
-      <c r="W30" s="7"/>
-      <c r="X30" s="7"/>
-      <c r="Y30" s="7"/>
-      <c r="Z30" s="7"/>
-      <c r="AA30" s="7"/>
-      <c r="AB30" s="7"/>
-      <c r="AC30" s="7"/>
-      <c r="AD30" s="7"/>
-      <c r="AE30" s="7"/>
-      <c r="AF30" s="7"/>
-      <c r="AG30" s="7"/>
-      <c r="AH30" s="32"/>
-      <c r="AI30" s="7"/>
-      <c r="AJ30" s="7"/>
-      <c r="AK30" s="7"/>
-      <c r="AL30" s="7"/>
-      <c r="AM30" s="7"/>
-      <c r="AN30" s="7"/>
-      <c r="AO30" s="7"/>
-      <c r="AP30" s="7"/>
-      <c r="AQ30" s="7"/>
-      <c r="AR30" s="7"/>
-      <c r="AS30" s="7"/>
-      <c r="AT30" s="7"/>
-      <c r="AU30" s="7"/>
-      <c r="AV30" s="7"/>
-      <c r="AW30" s="7"/>
-      <c r="AX30" s="7"/>
+      <c r="H30" s="7">
+        <v>0.5</v>
+      </c>
+      <c r="I30" s="7">
+        <v>3</v>
+      </c>
+      <c r="J30" s="7">
+        <v>1.5</v>
+      </c>
+      <c r="K30" s="7">
+        <v>2</v>
+      </c>
+      <c r="L30" s="7">
+        <v>2</v>
+      </c>
+      <c r="M30" s="7">
+        <v>2</v>
+      </c>
+      <c r="N30" s="7">
+        <v>3.5</v>
+      </c>
+      <c r="O30" s="7">
+        <v>2.5</v>
+      </c>
+      <c r="P30" s="7">
+        <v>1</v>
+      </c>
+      <c r="Q30" s="7">
+        <v>5</v>
+      </c>
+      <c r="R30" s="7">
+        <v>2</v>
+      </c>
+      <c r="S30" s="7">
+        <v>3</v>
+      </c>
+      <c r="T30" s="7">
+        <v>3</v>
+      </c>
+      <c r="U30" s="7">
+        <v>0</v>
+      </c>
+      <c r="V30" s="7">
+        <v>1.5</v>
+      </c>
+      <c r="W30" s="7">
+        <v>1</v>
+      </c>
+      <c r="X30" s="7">
+        <v>1</v>
+      </c>
+      <c r="Y30" s="7">
+        <v>1</v>
+      </c>
+      <c r="Z30" s="7">
+        <v>1</v>
+      </c>
+      <c r="AA30" s="7">
+        <v>1.5</v>
+      </c>
+      <c r="AB30" s="7">
+        <v>5</v>
+      </c>
+      <c r="AC30" s="7">
+        <v>2.5</v>
+      </c>
+      <c r="AD30" s="7">
+        <v>0</v>
+      </c>
+      <c r="AE30" s="7">
+        <v>0.5</v>
+      </c>
+      <c r="AF30" s="7">
+        <v>2</v>
+      </c>
+      <c r="AG30" s="7">
+        <v>2</v>
+      </c>
+      <c r="AH30" s="7">
+        <v>1</v>
+      </c>
+      <c r="AI30" s="7">
+        <v>0</v>
+      </c>
+      <c r="AJ30" s="7">
+        <v>1.5</v>
+      </c>
+      <c r="AK30" s="7">
+        <v>2</v>
+      </c>
+      <c r="AL30" s="7">
+        <v>0</v>
+      </c>
+      <c r="AM30" s="7">
+        <v>3.5</v>
+      </c>
+      <c r="AN30" s="7">
+        <v>1.5</v>
+      </c>
+      <c r="AO30" s="7">
+        <v>0</v>
+      </c>
+      <c r="AP30" s="7">
+        <v>1</v>
+      </c>
+      <c r="AQ30" s="7">
+        <v>1.5</v>
+      </c>
+      <c r="AR30" s="7">
+        <v>1.5</v>
+      </c>
+      <c r="AS30" s="7">
+        <v>0</v>
+      </c>
+      <c r="AT30" s="7">
+        <v>0</v>
+      </c>
+      <c r="AU30" s="7">
+        <v>2.5</v>
+      </c>
+      <c r="AV30" s="7">
+        <v>0.5</v>
+      </c>
+      <c r="AW30" s="7">
+        <v>2.5</v>
+      </c>
+      <c r="AX30" s="7">
+        <v>0</v>
+      </c>
       <c r="AY30" s="28"/>
       <c r="AZ30" s="28"/>
       <c r="BA30" s="1">
         <f t="shared" si="7"/>
-        <v>0</v>
+        <v>69</v>
       </c>
       <c r="BB30" s="1">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>6900</v>
       </c>
       <c r="BC30" s="1">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>-69</v>
       </c>
       <c r="BD30" s="1">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>-6900</v>
       </c>
     </row>
     <row r="31" spans="1:56">
@@ -5232,66 +5575,152 @@
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="H31" s="7"/>
-      <c r="I31" s="7"/>
-      <c r="J31" s="7"/>
-      <c r="K31" s="7"/>
-      <c r="L31" s="7"/>
-      <c r="M31" s="7"/>
-      <c r="N31" s="7"/>
-      <c r="O31" s="7"/>
-      <c r="P31" s="7"/>
-      <c r="Q31" s="7"/>
-      <c r="R31" s="7"/>
-      <c r="S31" s="7"/>
-      <c r="T31" s="7"/>
-      <c r="U31" s="7"/>
-      <c r="V31" s="7"/>
-      <c r="W31" s="7"/>
-      <c r="X31" s="7"/>
-      <c r="Y31" s="7"/>
-      <c r="Z31" s="7"/>
-      <c r="AA31" s="7"/>
-      <c r="AB31" s="7"/>
-      <c r="AC31" s="7"/>
-      <c r="AD31" s="7"/>
-      <c r="AE31" s="7"/>
-      <c r="AF31" s="7"/>
-      <c r="AG31" s="7"/>
-      <c r="AH31" s="32"/>
-      <c r="AI31" s="7"/>
-      <c r="AJ31" s="7"/>
-      <c r="AK31" s="7"/>
-      <c r="AL31" s="7"/>
-      <c r="AM31" s="7"/>
-      <c r="AN31" s="7"/>
-      <c r="AO31" s="7"/>
-      <c r="AP31" s="7"/>
-      <c r="AQ31" s="7"/>
-      <c r="AR31" s="7"/>
-      <c r="AS31" s="7"/>
-      <c r="AT31" s="7"/>
-      <c r="AU31" s="7"/>
-      <c r="AV31" s="7"/>
-      <c r="AW31" s="7"/>
-      <c r="AX31" s="7"/>
+      <c r="H31" s="7">
+        <v>0.5</v>
+      </c>
+      <c r="I31" s="7">
+        <v>3</v>
+      </c>
+      <c r="J31" s="7">
+        <v>1.5</v>
+      </c>
+      <c r="K31" s="7">
+        <v>2</v>
+      </c>
+      <c r="L31" s="7">
+        <v>2</v>
+      </c>
+      <c r="M31" s="7">
+        <v>2</v>
+      </c>
+      <c r="N31" s="7">
+        <v>3.5</v>
+      </c>
+      <c r="O31" s="7">
+        <v>2.5</v>
+      </c>
+      <c r="P31" s="7">
+        <v>1</v>
+      </c>
+      <c r="Q31" s="7">
+        <v>5</v>
+      </c>
+      <c r="R31" s="7">
+        <v>2</v>
+      </c>
+      <c r="S31" s="7">
+        <v>3</v>
+      </c>
+      <c r="T31" s="7">
+        <v>3</v>
+      </c>
+      <c r="U31" s="7">
+        <v>0</v>
+      </c>
+      <c r="V31" s="7">
+        <v>1.5</v>
+      </c>
+      <c r="W31" s="7">
+        <v>1</v>
+      </c>
+      <c r="X31" s="7">
+        <v>1</v>
+      </c>
+      <c r="Y31" s="7">
+        <v>1</v>
+      </c>
+      <c r="Z31" s="7">
+        <v>1</v>
+      </c>
+      <c r="AA31" s="7">
+        <v>0</v>
+      </c>
+      <c r="AB31" s="7">
+        <v>5</v>
+      </c>
+      <c r="AC31" s="7">
+        <v>2.5</v>
+      </c>
+      <c r="AD31" s="7">
+        <v>2</v>
+      </c>
+      <c r="AE31" s="7">
+        <v>0.5</v>
+      </c>
+      <c r="AF31" s="7">
+        <v>2</v>
+      </c>
+      <c r="AG31" s="7">
+        <v>2</v>
+      </c>
+      <c r="AH31" s="7">
+        <v>1</v>
+      </c>
+      <c r="AI31" s="7">
+        <v>1.5</v>
+      </c>
+      <c r="AJ31" s="7">
+        <v>1.5</v>
+      </c>
+      <c r="AK31" s="7">
+        <v>2</v>
+      </c>
+      <c r="AL31" s="7">
+        <v>3</v>
+      </c>
+      <c r="AM31" s="7">
+        <v>3.5</v>
+      </c>
+      <c r="AN31" s="7">
+        <v>1.5</v>
+      </c>
+      <c r="AO31" s="7">
+        <v>2</v>
+      </c>
+      <c r="AP31" s="7">
+        <v>1</v>
+      </c>
+      <c r="AQ31" s="7">
+        <v>1.5</v>
+      </c>
+      <c r="AR31" s="7">
+        <v>1.5</v>
+      </c>
+      <c r="AS31" s="7">
+        <v>2</v>
+      </c>
+      <c r="AT31" s="7">
+        <v>0</v>
+      </c>
+      <c r="AU31" s="7">
+        <v>2.5</v>
+      </c>
+      <c r="AV31" s="7">
+        <v>0.5</v>
+      </c>
+      <c r="AW31" s="7">
+        <v>2.5</v>
+      </c>
+      <c r="AX31" s="7">
+        <v>0</v>
+      </c>
       <c r="AY31" s="28"/>
       <c r="AZ31" s="28"/>
       <c r="BA31" s="1">
         <f t="shared" si="7"/>
-        <v>0</v>
+        <v>78</v>
       </c>
       <c r="BB31" s="1">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>7800</v>
       </c>
       <c r="BC31" s="1">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>-78</v>
       </c>
       <c r="BD31" s="1">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>-7800</v>
       </c>
     </row>
     <row r="32" spans="1:56" s="4" customFormat="1">
@@ -5301,55 +5730,55 @@
       </c>
       <c r="H32" s="4">
         <f t="shared" ref="H32:AW32" si="8">SUM(H2:H31)</f>
-        <v>12</v>
+        <v>14.5</v>
       </c>
       <c r="I32" s="4">
         <f t="shared" si="8"/>
-        <v>77.5</v>
+        <v>92.5</v>
       </c>
       <c r="J32" s="4">
         <f t="shared" si="8"/>
-        <v>37.5</v>
+        <v>45</v>
       </c>
       <c r="K32" s="4">
         <f t="shared" si="8"/>
-        <v>50</v>
+        <v>60</v>
       </c>
       <c r="L32" s="4">
         <f t="shared" si="8"/>
-        <v>44</v>
+        <v>60</v>
       </c>
       <c r="M32" s="4">
         <f t="shared" si="8"/>
-        <v>18</v>
+        <v>28</v>
       </c>
       <c r="N32" s="4">
         <f t="shared" si="8"/>
-        <v>15</v>
+        <v>32.5</v>
       </c>
       <c r="O32" s="4">
         <f t="shared" si="8"/>
-        <v>57.5</v>
+        <v>70</v>
       </c>
       <c r="P32" s="4">
         <f t="shared" si="8"/>
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="Q32" s="4">
         <f t="shared" si="8"/>
-        <v>125</v>
+        <v>150</v>
       </c>
       <c r="R32" s="4">
         <f t="shared" si="8"/>
-        <v>50</v>
+        <v>60</v>
       </c>
       <c r="S32" s="4">
         <f t="shared" si="8"/>
-        <v>76</v>
+        <v>91</v>
       </c>
       <c r="T32" s="4">
         <f t="shared" si="8"/>
-        <v>75</v>
+        <v>90</v>
       </c>
       <c r="U32" s="4">
         <f t="shared" si="8"/>
@@ -5357,99 +5786,99 @@
       </c>
       <c r="V32" s="4">
         <f t="shared" si="8"/>
-        <v>37.5</v>
+        <v>45</v>
       </c>
       <c r="W32" s="4">
         <f t="shared" si="8"/>
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="X32" s="4">
         <f t="shared" si="8"/>
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="Y32" s="4">
         <f t="shared" si="8"/>
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="Z32" s="4">
         <f t="shared" si="8"/>
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="AA32" s="4">
         <f t="shared" si="8"/>
-        <v>32.5</v>
+        <v>38.5</v>
       </c>
       <c r="AB32" s="4">
         <f t="shared" si="8"/>
-        <v>125</v>
+        <v>150</v>
       </c>
       <c r="AC32" s="4">
         <f t="shared" si="8"/>
-        <v>62.5</v>
+        <v>75</v>
       </c>
       <c r="AD32" s="4">
         <f t="shared" si="8"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AE32" s="4">
         <f t="shared" si="8"/>
-        <v>12.5</v>
+        <v>15</v>
       </c>
       <c r="AF32" s="4">
         <f t="shared" si="8"/>
-        <v>53</v>
+        <v>63</v>
       </c>
       <c r="AG32" s="4">
         <f t="shared" si="8"/>
-        <v>50</v>
+        <v>60</v>
       </c>
       <c r="AH32" s="4">
         <f t="shared" si="8"/>
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="AI32" s="4">
         <f t="shared" si="8"/>
-        <v>36</v>
+        <v>37.5</v>
       </c>
       <c r="AJ32" s="4">
         <f t="shared" si="8"/>
-        <v>37.5</v>
+        <v>45</v>
       </c>
       <c r="AK32" s="4">
         <f t="shared" si="8"/>
-        <v>85.5</v>
+        <v>95.5</v>
       </c>
       <c r="AL32" s="4">
         <f t="shared" si="8"/>
-        <v>72</v>
+        <v>81</v>
       </c>
       <c r="AM32" s="4">
         <f t="shared" si="8"/>
-        <v>87.5</v>
+        <v>105</v>
       </c>
       <c r="AN32" s="4">
         <f t="shared" si="8"/>
-        <v>37.5</v>
+        <v>45</v>
       </c>
       <c r="AO32" s="4">
         <f t="shared" si="8"/>
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="AP32" s="4">
         <f t="shared" si="8"/>
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="AQ32" s="4">
         <f t="shared" si="8"/>
-        <v>48</v>
+        <v>55.5</v>
       </c>
       <c r="AR32" s="4">
         <f t="shared" si="8"/>
-        <v>37.5</v>
+        <v>45</v>
       </c>
       <c r="AS32" s="4">
         <f t="shared" si="8"/>
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="AT32" s="4">
         <f t="shared" si="8"/>
@@ -5457,15 +5886,15 @@
       </c>
       <c r="AU32" s="4">
         <f t="shared" si="8"/>
-        <v>57.5</v>
+        <v>70</v>
       </c>
       <c r="AV32" s="4">
         <f t="shared" si="8"/>
-        <v>10</v>
+        <v>12.5</v>
       </c>
       <c r="AW32" s="4">
         <f t="shared" si="8"/>
-        <v>60.5</v>
+        <v>73</v>
       </c>
       <c r="AY32" s="4">
         <f>SUM(AY2:AY31)</f>
@@ -5477,19 +5906,19 @@
       </c>
       <c r="BA32" s="4">
         <f>SUM(BA2:BA31)</f>
-        <v>1847</v>
+        <v>2215</v>
       </c>
       <c r="BB32" s="4">
         <f>SUM(BB2:BB31)</f>
-        <v>184700</v>
+        <v>221500</v>
       </c>
       <c r="BC32" s="4">
         <f>SUM(BC2:BC29)</f>
-        <v>-1744.5</v>
+        <v>-1965.5</v>
       </c>
       <c r="BD32" s="4">
         <f>SUM(BD2:BD29)</f>
-        <v>-184597.5</v>
+        <v>-206697.5</v>
       </c>
     </row>
     <row r="33" spans="1:53" s="10" customFormat="1">
@@ -5498,55 +5927,55 @@
       </c>
       <c r="H33" s="10">
         <f>H32*90</f>
-        <v>1080</v>
+        <v>1305</v>
       </c>
       <c r="I33" s="10">
         <f>I32*120</f>
-        <v>9300</v>
+        <v>11100</v>
       </c>
       <c r="J33" s="10">
         <f>J32*120</f>
-        <v>4500</v>
+        <v>5400</v>
       </c>
       <c r="K33" s="10">
         <f>K32*110</f>
-        <v>5500</v>
+        <v>6600</v>
       </c>
       <c r="L33" s="10">
         <f>L32*120</f>
-        <v>5280</v>
+        <v>7200</v>
       </c>
       <c r="M33" s="10">
         <f>M32*100</f>
-        <v>1800</v>
+        <v>2800</v>
       </c>
       <c r="N33" s="10">
         <f>N32*100</f>
-        <v>1500</v>
+        <v>3250</v>
       </c>
       <c r="O33" s="10">
         <f>O32*120</f>
-        <v>6900</v>
+        <v>8400</v>
       </c>
       <c r="P33" s="10">
         <f>P32*100</f>
-        <v>2500</v>
+        <v>3000</v>
       </c>
       <c r="Q33" s="10">
         <f>Q32*120</f>
-        <v>15000</v>
+        <v>18000</v>
       </c>
       <c r="R33" s="10">
         <f t="shared" ref="R33:U33" si="9">R32*120</f>
-        <v>6000</v>
+        <v>7200</v>
       </c>
       <c r="S33" s="10">
         <f>S32*120</f>
-        <v>9120</v>
+        <v>10920</v>
       </c>
       <c r="T33" s="10">
         <f>T32*120</f>
-        <v>9000</v>
+        <v>10800</v>
       </c>
       <c r="U33" s="10">
         <f t="shared" si="9"/>
@@ -5554,99 +5983,99 @@
       </c>
       <c r="V33" s="10">
         <f>V32*110</f>
-        <v>4125</v>
+        <v>4950</v>
       </c>
       <c r="W33" s="10">
         <f>W32*120</f>
-        <v>3000</v>
+        <v>3600</v>
       </c>
       <c r="X33" s="10">
         <f>X32*110</f>
-        <v>2750</v>
+        <v>3300</v>
       </c>
       <c r="Y33" s="10">
         <f>Y32*100</f>
-        <v>2500</v>
+        <v>3000</v>
       </c>
       <c r="Z33" s="10">
         <f>Z32*100</f>
-        <v>2500</v>
+        <v>3000</v>
       </c>
       <c r="AA33" s="10">
         <f>AA32*110</f>
-        <v>3575</v>
+        <v>4235</v>
       </c>
       <c r="AB33" s="11">
         <f>AB32*120</f>
-        <v>15000</v>
+        <v>18000</v>
       </c>
       <c r="AC33" s="11">
         <f>AC32*100</f>
-        <v>6250</v>
+        <v>7500</v>
       </c>
       <c r="AD33" s="11">
         <f>AD32*100</f>
-        <v>0</v>
+        <v>200</v>
       </c>
       <c r="AE33" s="11">
         <f>AE32*110</f>
-        <v>1375</v>
+        <v>1650</v>
       </c>
       <c r="AF33" s="11">
         <f>AF32*110</f>
-        <v>5830</v>
+        <v>6930</v>
       </c>
       <c r="AG33" s="12">
         <f>AG32*110</f>
-        <v>5500</v>
+        <v>6600</v>
       </c>
       <c r="AH33" s="11">
         <f>AH32*110</f>
-        <v>2750</v>
+        <v>3300</v>
       </c>
       <c r="AI33" s="11">
         <f>AI32*120</f>
-        <v>4320</v>
+        <v>4500</v>
       </c>
       <c r="AJ33" s="11">
         <f>AJ32*120</f>
-        <v>4500</v>
+        <v>5400</v>
       </c>
       <c r="AK33" s="11">
         <f>AK32*120</f>
-        <v>10260</v>
+        <v>11460</v>
       </c>
       <c r="AL33" s="11">
         <f>AL32*120</f>
-        <v>8640</v>
+        <v>9720</v>
       </c>
       <c r="AM33" s="11">
         <f t="shared" ref="AM33" si="10">AM32*120</f>
-        <v>10500</v>
+        <v>12600</v>
       </c>
       <c r="AN33" s="11">
         <f>AN32*120</f>
-        <v>4500</v>
+        <v>5400</v>
       </c>
       <c r="AO33" s="11">
         <f>AO32*120</f>
-        <v>1080</v>
+        <v>1320</v>
       </c>
       <c r="AP33" s="11">
         <f>AP32*120</f>
-        <v>3000</v>
+        <v>3600</v>
       </c>
       <c r="AQ33" s="11">
         <f>AQ32*120</f>
-        <v>5760</v>
+        <v>6660</v>
       </c>
       <c r="AR33" s="11">
         <f>AR32*110</f>
-        <v>4125</v>
+        <v>4950</v>
       </c>
       <c r="AS33" s="11">
         <f>AS32*120</f>
-        <v>2640</v>
+        <v>3120</v>
       </c>
       <c r="AT33" s="11">
         <f>AT32*110</f>
@@ -5654,15 +6083,15 @@
       </c>
       <c r="AU33" s="11">
         <f>AU32*120</f>
-        <v>6900</v>
+        <v>8400</v>
       </c>
       <c r="AV33" s="11">
         <f>AV32*120</f>
-        <v>1200</v>
+        <v>1500</v>
       </c>
       <c r="AW33" s="11">
         <f>AW32*120</f>
-        <v>7260</v>
+        <v>8760</v>
       </c>
       <c r="AX33" s="11"/>
       <c r="AY33" s="11">
@@ -5675,7 +6104,7 @@
       </c>
       <c r="BA33" s="9">
         <f>SUM(H33:AZ33)</f>
-        <v>213950</v>
+        <v>256260</v>
       </c>
     </row>
     <row r="34" spans="1:53" s="13" customFormat="1">
@@ -6109,55 +6538,55 @@
       </c>
       <c r="H37" s="17">
         <f>(H36+H35)-(H33+H34)</f>
-        <v>-1080</v>
+        <v>-1305</v>
       </c>
       <c r="I37" s="17">
         <f>(I36+I35)-(I33+I34)</f>
-        <v>-9300</v>
+        <v>-11100</v>
       </c>
       <c r="J37" s="17">
         <f t="shared" ref="J37:BA37" si="11">(J36+J35)-(J33+J34)</f>
-        <v>-4500</v>
+        <v>-5400</v>
       </c>
       <c r="K37" s="17">
         <f t="shared" si="11"/>
-        <v>-5500</v>
+        <v>-6600</v>
       </c>
       <c r="L37" s="17">
         <f t="shared" si="11"/>
-        <v>-5280</v>
+        <v>-7200</v>
       </c>
       <c r="M37" s="17">
         <f t="shared" si="11"/>
-        <v>-1800</v>
+        <v>-2800</v>
       </c>
       <c r="N37" s="17">
         <f t="shared" si="11"/>
-        <v>-1500</v>
+        <v>-3250</v>
       </c>
       <c r="O37" s="17">
         <f t="shared" si="11"/>
-        <v>-6900</v>
+        <v>-8400</v>
       </c>
       <c r="P37" s="17">
         <f t="shared" si="11"/>
-        <v>500</v>
+        <v>0</v>
       </c>
       <c r="Q37" s="17">
         <f t="shared" si="11"/>
-        <v>-15000</v>
+        <v>-18000</v>
       </c>
       <c r="R37" s="17">
         <f t="shared" si="11"/>
-        <v>-6000</v>
+        <v>-7200</v>
       </c>
       <c r="S37" s="17">
         <f t="shared" si="11"/>
-        <v>-9120</v>
+        <v>-10920</v>
       </c>
       <c r="T37" s="17">
         <f t="shared" si="11"/>
-        <v>-9000</v>
+        <v>-10800</v>
       </c>
       <c r="U37" s="17">
         <f t="shared" si="11"/>
@@ -6165,99 +6594,99 @@
       </c>
       <c r="V37" s="17">
         <f t="shared" si="11"/>
-        <v>-4125</v>
+        <v>-4950</v>
       </c>
       <c r="W37" s="17">
         <f t="shared" si="11"/>
-        <v>-3000</v>
+        <v>-3600</v>
       </c>
       <c r="X37" s="17">
         <f t="shared" si="11"/>
-        <v>-2750</v>
+        <v>-3300</v>
       </c>
       <c r="Y37" s="17">
         <f t="shared" si="11"/>
-        <v>-2500</v>
+        <v>-3000</v>
       </c>
       <c r="Z37" s="17">
         <f t="shared" si="11"/>
-        <v>-2500</v>
+        <v>-3000</v>
       </c>
       <c r="AA37" s="17">
         <f t="shared" si="11"/>
-        <v>-3575</v>
+        <v>-4235</v>
       </c>
       <c r="AB37" s="17">
         <f t="shared" si="11"/>
-        <v>-15000</v>
+        <v>-18000</v>
       </c>
       <c r="AC37" s="17">
         <f t="shared" si="11"/>
-        <v>-6250</v>
+        <v>-7500</v>
       </c>
       <c r="AD37" s="17">
         <f t="shared" si="11"/>
-        <v>0</v>
+        <v>-200</v>
       </c>
       <c r="AE37" s="17">
         <f t="shared" si="11"/>
-        <v>-1375</v>
+        <v>-1650</v>
       </c>
       <c r="AF37" s="17">
         <f t="shared" si="11"/>
-        <v>-5830</v>
+        <v>-6930</v>
       </c>
       <c r="AG37" s="17">
         <f t="shared" si="11"/>
-        <v>-5500</v>
+        <v>-6600</v>
       </c>
       <c r="AH37" s="17">
         <f t="shared" si="11"/>
-        <v>-2750</v>
+        <v>-3300</v>
       </c>
       <c r="AI37" s="17">
         <f t="shared" si="11"/>
-        <v>-4320</v>
+        <v>-4500</v>
       </c>
       <c r="AJ37" s="17">
         <f t="shared" si="11"/>
-        <v>-14565</v>
+        <v>-15465</v>
       </c>
       <c r="AK37" s="17">
         <f t="shared" si="11"/>
-        <v>-10260</v>
+        <v>-11460</v>
       </c>
       <c r="AL37" s="17">
         <f t="shared" si="11"/>
-        <v>-8640</v>
+        <v>-9720</v>
       </c>
       <c r="AM37" s="17">
         <f t="shared" si="11"/>
-        <v>-10500</v>
+        <v>-12600</v>
       </c>
       <c r="AN37" s="17">
         <f t="shared" si="11"/>
-        <v>-4500</v>
+        <v>-5400</v>
       </c>
       <c r="AO37" s="17">
         <f t="shared" si="11"/>
-        <v>-1080</v>
+        <v>-1320</v>
       </c>
       <c r="AP37" s="17">
         <f t="shared" si="11"/>
-        <v>-3000</v>
+        <v>-3600</v>
       </c>
       <c r="AQ37" s="17">
         <f t="shared" si="11"/>
-        <v>-5760</v>
+        <v>-6660</v>
       </c>
       <c r="AR37" s="17">
         <f t="shared" si="11"/>
-        <v>-4125</v>
+        <v>-4950</v>
       </c>
       <c r="AS37" s="17">
         <f t="shared" si="11"/>
-        <v>-2640</v>
+        <v>-3120</v>
       </c>
       <c r="AT37" s="17">
         <f t="shared" si="11"/>
@@ -6265,15 +6694,15 @@
       </c>
       <c r="AU37" s="17">
         <f t="shared" si="11"/>
-        <v>-6900</v>
+        <v>-8400</v>
       </c>
       <c r="AV37" s="17">
         <f t="shared" si="11"/>
-        <v>-1200</v>
+        <v>-1500</v>
       </c>
       <c r="AW37" s="17">
         <f t="shared" si="11"/>
-        <v>-7260</v>
+        <v>-8760</v>
       </c>
       <c r="AY37" s="17">
         <f>(AY36+AY35)-(AY33+AY34)</f>
@@ -6285,7 +6714,7 @@
       </c>
       <c r="BA37" s="18">
         <f t="shared" si="11"/>
-        <v>-224015</v>
+        <v>-266325</v>
       </c>
     </row>
     <row r="39" spans="1:53">

</xml_diff>